<commit_message>
Show all options with no answer. show questions one by one. pdf ok working on excel export
</commit_message>
<xml_diff>
--- a/public/Survey two.xlsx
+++ b/public/Survey two.xlsx
@@ -53,24 +53,24 @@
     <t>All multiple question 1</t>
   </si>
   <si>
+    <t>jjjhjhjh</t>
+  </si>
+  <si>
+    <t>jfghfjghjfdhg fghfjg</t>
+  </si>
+  <si>
+    <t>khjkjhj jkjhjhkhj</t>
+  </si>
+  <si>
+    <t>Forth answer</t>
+  </si>
+  <si>
     <t>ghghg</t>
   </si>
   <si>
     <t>hghgh</t>
   </si>
   <si>
-    <t>jjjhjhjh</t>
-  </si>
-  <si>
-    <t>jfghfjghjfdhg fghfjg</t>
-  </si>
-  <si>
-    <t>khjkjhj jkjhjhkhj</t>
-  </si>
-  <si>
-    <t>Forth answer</t>
-  </si>
-  <si>
     <t>New text option question</t>
   </si>
   <si>
@@ -80,10 +80,10 @@
     <t>test text</t>
   </si>
   <si>
+    <t>hghghjhg</t>
+  </si>
+  <si>
     <t>jgg</t>
-  </si>
-  <si>
-    <t>hghghjhg</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="30" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -505,7 +505,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -594,6 +594,31 @@
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A9:A9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A15:A15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A17:A17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A17:A18"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
sort by question. all option ok
</commit_message>
<xml_diff>
--- a/public/Survey two.xlsx
+++ b/public/Survey two.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Question name</t>
   </si>
@@ -26,64 +26,100 @@
     <t>Total</t>
   </si>
   <si>
+    <t>test question</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>no comment</t>
+  </si>
+  <si>
+    <t>test text</t>
+  </si>
+  <si>
+    <t>jdkhfjdsfhj</t>
+  </si>
+  <si>
+    <t>djhfjhdsjfhdsf</t>
+  </si>
+  <si>
+    <t>dmfdsmfnsd</t>
+  </si>
+  <si>
+    <t>New text option question</t>
+  </si>
+  <si>
+    <t>ffjhjhsdjhfjsdhf</t>
+  </si>
+  <si>
+    <t>djfhsdjf fdjhsdjhf</t>
+  </si>
+  <si>
+    <t>fkjkhf sdjfbsjdkhf</t>
+  </si>
+  <si>
+    <t>hhghghghg</t>
+  </si>
+  <si>
+    <t>No answer</t>
+  </si>
+  <si>
+    <t>Updated question</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>new kfhfhkhd</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>All multiple question 3</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Option 3</t>
+  </si>
+  <si>
+    <t>All multiple question 2</t>
+  </si>
+  <si>
+    <t>All multiple question 1</t>
+  </si>
+  <si>
+    <t>jdfhdjsfhjsdhf</t>
+  </si>
+  <si>
+    <t>dfjhdjsd fksjdhfjksd</t>
+  </si>
+  <si>
+    <t>mdfd fsdjbfjsdhfjhsdf</t>
+  </si>
+  <si>
     <t>Question two?</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>NO COMMENT</t>
   </si>
   <si>
-    <t>All multiple question 2</t>
-  </si>
-  <si>
-    <t>Option 1</t>
-  </si>
-  <si>
-    <t>Option 3</t>
-  </si>
-  <si>
-    <t>Updated question</t>
-  </si>
-  <si>
-    <t>All multiple question 1</t>
-  </si>
-  <si>
-    <t>jjjhjhjh</t>
-  </si>
-  <si>
-    <t>jfghfjghjfdhg fghfjg</t>
-  </si>
-  <si>
-    <t>khjkjhj jkjhjhkhj</t>
-  </si>
-  <si>
-    <t>Forth answer</t>
-  </si>
-  <si>
-    <t>ghghg</t>
-  </si>
-  <si>
-    <t>hghgh</t>
-  </si>
-  <si>
-    <t>New text option question</t>
-  </si>
-  <si>
-    <t>hhghhjgjh hvbvbbv</t>
-  </si>
-  <si>
-    <t>test text</t>
-  </si>
-  <si>
-    <t>hghghjhg</t>
-  </si>
-  <si>
-    <t>jgg</t>
+    <t>Another</t>
   </si>
 </sst>
 </file>
@@ -440,7 +476,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C1" sqref="C1"/>
@@ -467,7 +503,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -476,7 +512,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -485,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -495,129 +531,236 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
+      <c r="C5"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6"/>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
+      <c r="C6"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7"/>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
+      <c r="C7"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9"/>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C10"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11"/>
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C11"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12"/>
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14"/>
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
+      <c r="A15"/>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16"/>
-      <c r="B16"/>
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
+      <c r="A17"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20"/>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23"/>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24"/>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26"/>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27"/>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28"/>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A9:A9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A15:A15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A17:A17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A11:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A28"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>